<commit_message>
Changed Full Frame to Full-Frame
</commit_message>
<xml_diff>
--- a/BigAssTableOfImagingFormats.xlsx
+++ b/BigAssTableOfImagingFormats.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableofImagingFormats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbruggeman/Documents/MTFWServer/BigAssTableOfImagingFormats/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="17260" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="BigAssTableOfImagingFormats" sheetId="1" r:id="rId1"/>
     <sheet name="Changelog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Format</t>
   </si>
@@ -51,9 +57,6 @@
     <t>1"</t>
   </si>
   <si>
-    <t>Full Frame</t>
-  </si>
-  <si>
     <t>Super 35</t>
   </si>
   <si>
@@ -100,12 +103,18 @@
   </si>
   <si>
     <t>Initial Commit, bulk of digital and film formats</t>
+  </si>
+  <si>
+    <t>Changed "Full Frame" to "Full-Frame" to match BATOL</t>
+  </si>
+  <si>
+    <t>Full-Frame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,16 +495,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,15 +518,15 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -538,7 +547,7 @@
         <v>21.633307652783937</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -561,7 +570,7 @@
         <v>14.144963768069539</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -584,7 +593,7 @@
         <v>16.765813430907549</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -607,7 +616,7 @@
         <v>10.820004621071103</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -630,9 +639,9 @@
         <v>7.9322128060207762</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>22</v>
@@ -653,9 +662,9 @@
         <v>13.601470508735444</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>12.52</v>
@@ -676,9 +685,9 @@
         <v>7.2742439469679594</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>5.79</v>
@@ -699,9 +708,9 @@
         <v>3.5215124591572864</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>44</v>
@@ -722,9 +731,9 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>53.7</v>
@@ -745,9 +754,9 @@
         <v>33.540013416813061</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>56</v>
@@ -768,9 +777,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>56</v>
@@ -791,9 +800,9 @@
         <v>39.597979746446661</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>67</v>
@@ -814,9 +823,9 @@
         <v>43.660622991432454</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>70.41</v>
@@ -837,9 +846,9 @@
         <v>43.953057345308757</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>121</v>
@@ -860,9 +869,9 @@
         <v>77.540312096354114</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>178</v>
@@ -883,9 +892,9 @@
         <v>109.33091968880532</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>254</v>
@@ -916,27 +925,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42814</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>42815</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Full-Circle imaging format
</commit_message>
<xml_diff>
--- a/BigAssTableOfImagingFormats.xlsx
+++ b/BigAssTableOfImagingFormats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="17260" windowHeight="12660"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="17260" windowHeight="12660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BigAssTableOfImagingFormats" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Format</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Full-Frame</t>
+  </si>
+  <si>
+    <t>Full-Circle</t>
+  </si>
+  <si>
+    <t>Added "Full-Circle" format for complete data visualization</t>
   </si>
 </sst>
 </file>
@@ -176,8 +182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Format"/>
     <tableColumn id="2" name="Width (mm)"/>
@@ -493,9 +499,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -526,391 +532,414 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>864</v>
-      </c>
-      <c r="E2">
-        <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.5</v>
-      </c>
-      <c r="F2">
-        <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>21.633307652783937</v>
+        <v>40</v>
+      </c>
+      <c r="D2" s="1">
+        <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
+        <v>1600</v>
+      </c>
+      <c r="E2" s="1">
+        <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
+        <v>28.284271247461902</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>23.6</v>
+        <v>36</v>
       </c>
       <c r="C3">
-        <v>15.6</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>368.16</v>
+        <v>864</v>
       </c>
       <c r="E3">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.512820512820513</v>
+        <v>1.5</v>
       </c>
       <c r="F3">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>14.144963768069539</v>
+        <v>21.633307652783937</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>27.9</v>
+        <v>23.6</v>
       </c>
       <c r="C4">
-        <v>18.600000000000001</v>
+        <v>15.6</v>
       </c>
       <c r="D4">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>518.94000000000005</v>
+        <v>368.16</v>
       </c>
       <c r="E4">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.4999999999999998</v>
+        <v>1.512820512820513</v>
       </c>
       <c r="F4">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>16.765813430907549</v>
+        <v>14.144963768069539</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>17.3</v>
+        <v>27.9</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="D5">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>224.9</v>
+        <v>518.94000000000005</v>
       </c>
       <c r="E5">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.3307692307692309</v>
+        <v>1.4999999999999998</v>
       </c>
       <c r="F5">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>10.820004621071103</v>
+        <v>16.765813430907549</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>13.2</v>
+        <v>17.3</v>
       </c>
       <c r="C6">
-        <v>8.8000000000000007</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>116.16</v>
+        <v>224.9</v>
       </c>
       <c r="E6">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.4999999999999998</v>
+        <v>1.3307692307692309</v>
       </c>
       <c r="F6">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>7.9322128060207762</v>
+        <v>10.820004621071103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>13.2</v>
       </c>
       <c r="C7">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1">
-        <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>352</v>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D7">
+        <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
+        <v>116.16</v>
       </c>
       <c r="E7">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.375</v>
+        <v>1.4999999999999998</v>
       </c>
       <c r="F7">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>13.601470508735444</v>
+        <v>7.9322128060207762</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>12.52</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>7.41</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>92.773200000000003</v>
+        <v>352</v>
       </c>
       <c r="E8">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.689608636977058</v>
+        <v>1.375</v>
       </c>
       <c r="F8">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>7.2742439469679594</v>
+        <v>13.601470508735444</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>5.79</v>
+        <v>12.52</v>
       </c>
       <c r="C9">
-        <v>4.01</v>
+        <v>7.41</v>
       </c>
       <c r="D9" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>23.2179</v>
+        <v>92.773200000000003</v>
       </c>
       <c r="E9">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.4438902743142146</v>
+        <v>1.689608636977058</v>
       </c>
       <c r="F9">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>3.5215124591572864</v>
+        <v>7.2742439469679594</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>44</v>
+        <v>5.79</v>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>4.01</v>
       </c>
       <c r="D10" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>1452</v>
-      </c>
-      <c r="E10" s="1">
-        <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="F10" s="1">
-        <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>27.5</v>
+        <v>23.2179</v>
+      </c>
+      <c r="E10">
+        <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
+        <v>1.4438902743142146</v>
+      </c>
+      <c r="F10">
+        <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
+        <v>3.5215124591572864</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>53.7</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>40.200000000000003</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>2158.7400000000002</v>
+        <v>1452</v>
       </c>
       <c r="E11" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.335820895522388</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F11" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>33.540013416813061</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>53.7</v>
       </c>
       <c r="C12">
-        <v>42</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="D12" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>2352</v>
+        <v>2158.7400000000002</v>
       </c>
       <c r="E12" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.3333333333333333</v>
+        <v>1.335820895522388</v>
       </c>
       <c r="F12" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>35</v>
+        <v>33.540013416813061</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>56</v>
       </c>
       <c r="C13">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>3136</v>
+        <v>2352</v>
       </c>
       <c r="E13" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F13" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>39.597979746446661</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>56</v>
       </c>
       <c r="D14" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>3752</v>
+        <v>3136</v>
       </c>
       <c r="E14" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.1964285714285714</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>43.660622991432454</v>
+        <v>39.597979746446661</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>70.41</v>
+        <v>67</v>
       </c>
       <c r="C15">
-        <v>52.63</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>3705.6783</v>
+        <v>3752</v>
       </c>
       <c r="E15" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.3378301349040469</v>
+        <v>1.1964285714285714</v>
       </c>
       <c r="F15" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>43.953057345308757</v>
+        <v>43.660622991432454</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>121</v>
+        <v>70.41</v>
       </c>
       <c r="C16">
-        <v>97</v>
+        <v>52.63</v>
       </c>
       <c r="D16" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>11737</v>
+        <v>3705.6783</v>
       </c>
       <c r="E16" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.2474226804123711</v>
+        <v>1.3378301349040469</v>
       </c>
       <c r="F16" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>77.540312096354114</v>
+        <v>43.953057345308757</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>178</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="D17" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
-        <v>22606</v>
+        <v>11737</v>
       </c>
       <c r="E17" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
-        <v>1.4015748031496063</v>
+        <v>1.2474226804123711</v>
       </c>
       <c r="F17" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
-        <v>109.33091968880532</v>
+        <v>77.540312096354114</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>178</v>
+      </c>
+      <c r="C18">
+        <v>127</v>
+      </c>
+      <c r="D18" s="1">
+        <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
+        <v>22606</v>
+      </c>
+      <c r="E18" s="1">
+        <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
+        <v>1.4015748031496063</v>
+      </c>
+      <c r="F18" s="1">
+        <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
+        <v>109.33091968880532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>254</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>203</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <f>Table1[[#This Row],[Height (mm)]]*Table1[[#This Row],[Width (mm)]]</f>
         <v>51562</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <f>Table1[[#This Row],[Width (mm)]]/Table1[[#This Row],[Height (mm)]]</f>
         <v>1.2512315270935961</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <f>SQRT(Table1[[#This Row],[Width (mm)]]^2 +Table1[[#This Row],[Height (mm)]]^2)/2</f>
         <v>162.5769048788911</v>
       </c>
@@ -925,10 +954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -957,6 +986,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>42956</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>